<commit_message>
Fix: Update Apps Script URLs and timestamp format issue
- Update Shift A URL to: AKfycbyR-lhvK05GP1c4yRPuVwYPjEhElGCNGsumidY3pIY-b2qSN5EFLckWpL6hWz5MABA9
- Update Shift B URL to: AKfycbyMPKpqHRkrBggiTcnUgJzjQMYrlo53m5xnPz03jqo51vFny53BDw0S18BHdDqU4mms
- Fix timestamp format: Use Utilities.formatDate() instead of toLocaleString()
- Add validateAndRepairHeaders() for auto-repair corrupted headers
- Update documentation files (APPS-SCRIPT-URLS.md, DEPLOYMENT-SUMMARY.md)
</commit_message>
<xml_diff>
--- a/QR-tracking/รายงานสินค้าสำเร็จรูป.xlsx
+++ b/QR-tracking/รายงานสินค้าสำเร็จรูป.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zola Polysack\Desktop\V5.04 PD2_Shift-Combined\QR-tracking\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E7602B1C-FF83-4DDD-B454-5345B6B146EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FEE620DD-8E0F-4CD5-8B01-2FBDC662660E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="861" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="348" yWindow="348" windowWidth="2388" windowHeight="564" tabRatio="861" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ฟรอมร์" sheetId="182" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -703,7 +704,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -762,60 +763,177 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="justify"/>
     </xf>
@@ -824,138 +942,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="justify"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1337,7 +1323,7 @@
   <dimension ref="A1:AC67"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L35" sqref="L35"/>
+      <selection activeCell="I31" sqref="I31:L31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="16.95" customHeight="1"/>
@@ -1361,31 +1347,31 @@
       <c r="A1" s="3"/>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="76"/>
-      <c r="I1" s="78" t="s">
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
+      <c r="G1" s="58"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="26" t="s">
         <v>71</v>
       </c>
-      <c r="J1" s="79"/>
-      <c r="K1" s="79"/>
-      <c r="L1" s="79"/>
+      <c r="J1" s="76"/>
+      <c r="K1" s="76"/>
+      <c r="L1" s="76"/>
     </row>
     <row r="2" spans="1:23" ht="16.95" customHeight="1">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="76"/>
-      <c r="I2" s="78"/>
-      <c r="J2" s="79"/>
-      <c r="K2" s="79"/>
-      <c r="L2" s="79"/>
+      <c r="D2" s="58"/>
+      <c r="E2" s="58"/>
+      <c r="F2" s="58"/>
+      <c r="G2" s="58"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="26"/>
+      <c r="J2" s="76"/>
+      <c r="K2" s="76"/>
+      <c r="L2" s="76"/>
     </row>
     <row r="3" spans="1:23" ht="16.95" customHeight="1">
       <c r="A3" s="5"/>
@@ -1397,25 +1383,25 @@
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
       <c r="I3" s="6"/>
-      <c r="J3" s="33"/>
-      <c r="K3" s="33"/>
-      <c r="L3" s="33"/>
+      <c r="J3" s="77"/>
+      <c r="K3" s="77"/>
+      <c r="L3" s="77"/>
     </row>
     <row r="4" spans="1:23" s="8" customFormat="1" ht="24" customHeight="1">
-      <c r="A4" s="34" t="s">
+      <c r="A4" s="78" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="34"/>
-      <c r="C4" s="34"/>
-      <c r="D4" s="34"/>
-      <c r="E4" s="34"/>
-      <c r="F4" s="34"/>
-      <c r="G4" s="34"/>
-      <c r="H4" s="34"/>
-      <c r="I4" s="34"/>
-      <c r="J4" s="34"/>
-      <c r="K4" s="34"/>
-      <c r="L4" s="34"/>
+      <c r="B4" s="78"/>
+      <c r="C4" s="78"/>
+      <c r="D4" s="78"/>
+      <c r="E4" s="78"/>
+      <c r="F4" s="78"/>
+      <c r="G4" s="78"/>
+      <c r="H4" s="78"/>
+      <c r="I4" s="78"/>
+      <c r="J4" s="78"/>
+      <c r="K4" s="78"/>
+      <c r="L4" s="78"/>
     </row>
     <row r="5" spans="1:23" s="8" customFormat="1" ht="11.4" customHeight="1">
       <c r="A5" s="7"/>
@@ -1432,35 +1418,35 @@
       <c r="L5" s="7"/>
     </row>
     <row r="6" spans="1:23" s="8" customFormat="1" ht="20.399999999999999" customHeight="1">
-      <c r="A6" s="38" t="s">
+      <c r="A6" s="64" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="39"/>
-      <c r="C6" s="39"/>
-      <c r="D6" s="39"/>
-      <c r="E6" s="39"/>
-      <c r="F6" s="39"/>
-      <c r="G6" s="39"/>
-      <c r="H6" s="39"/>
-      <c r="I6" s="40" t="s">
+      <c r="B6" s="65"/>
+      <c r="C6" s="65"/>
+      <c r="D6" s="65"/>
+      <c r="E6" s="65"/>
+      <c r="F6" s="65"/>
+      <c r="G6" s="65"/>
+      <c r="H6" s="65"/>
+      <c r="I6" s="79" t="s">
         <v>2</v>
       </c>
-      <c r="J6" s="41"/>
-      <c r="K6" s="41"/>
-      <c r="L6" s="42"/>
-      <c r="R6" s="37"/>
-      <c r="S6" s="37"/>
-      <c r="T6" s="37"/>
-      <c r="U6" s="37"/>
-      <c r="V6" s="37"/>
-      <c r="W6" s="37"/>
+      <c r="J6" s="80"/>
+      <c r="K6" s="80"/>
+      <c r="L6" s="81"/>
+      <c r="R6" s="58"/>
+      <c r="S6" s="58"/>
+      <c r="T6" s="58"/>
+      <c r="U6" s="58"/>
+      <c r="V6" s="58"/>
+      <c r="W6" s="58"/>
     </row>
     <row r="7" spans="1:23" s="8" customFormat="1" ht="21.75" customHeight="1">
       <c r="A7" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="B7" s="78"/>
-      <c r="C7" s="78"/>
+      <c r="B7" s="26"/>
+      <c r="C7" s="26"/>
       <c r="D7" s="2" t="s">
         <v>65</v>
       </c>
@@ -1470,81 +1456,81 @@
         <v>72</v>
       </c>
       <c r="H7" s="2"/>
-      <c r="I7" s="77" t="s">
+      <c r="I7" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="J7" s="26"/>
-      <c r="K7" s="26"/>
-      <c r="L7" s="45"/>
-      <c r="R7" s="37"/>
-      <c r="S7" s="37"/>
-      <c r="T7" s="37"/>
-      <c r="U7" s="37"/>
-      <c r="V7" s="37"/>
-      <c r="W7" s="37"/>
+      <c r="J7" s="41"/>
+      <c r="K7" s="41"/>
+      <c r="L7" s="42"/>
+      <c r="R7" s="58"/>
+      <c r="S7" s="58"/>
+      <c r="T7" s="58"/>
+      <c r="U7" s="58"/>
+      <c r="V7" s="58"/>
+      <c r="W7" s="58"/>
     </row>
     <row r="8" spans="1:23" s="8" customFormat="1" ht="21.75" customHeight="1">
       <c r="A8" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="B8" s="28"/>
-      <c r="C8" s="28"/>
-      <c r="D8" s="24" t="s">
+      <c r="B8" s="27"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="39" t="s">
         <v>73</v>
       </c>
-      <c r="E8" s="24"/>
-      <c r="F8" s="24"/>
+      <c r="E8" s="39"/>
+      <c r="F8" s="39"/>
       <c r="G8" s="2" t="s">
         <v>58</v>
       </c>
       <c r="H8" s="2"/>
-      <c r="I8" s="47"/>
-      <c r="J8" s="32"/>
-      <c r="K8" s="32"/>
-      <c r="L8" s="48"/>
+      <c r="I8" s="70"/>
+      <c r="J8" s="71"/>
+      <c r="K8" s="71"/>
+      <c r="L8" s="72"/>
       <c r="M8" s="8" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:23" s="8" customFormat="1" ht="21" customHeight="1">
-      <c r="A9" s="84" t="s">
+      <c r="A9" s="25" t="s">
         <v>60</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D9" s="24" t="s">
+      <c r="D9" s="39" t="s">
         <v>51</v>
       </c>
-      <c r="E9" s="24"/>
-      <c r="F9" s="24"/>
+      <c r="E9" s="39"/>
+      <c r="F9" s="39"/>
       <c r="G9" s="2" t="s">
         <v>59</v>
       </c>
       <c r="H9" s="2"/>
-      <c r="I9" s="47"/>
-      <c r="J9" s="32"/>
-      <c r="K9" s="32"/>
-      <c r="L9" s="48"/>
+      <c r="I9" s="70"/>
+      <c r="J9" s="71"/>
+      <c r="K9" s="71"/>
+      <c r="L9" s="72"/>
     </row>
     <row r="10" spans="1:23" s="8" customFormat="1" ht="21" customHeight="1">
-      <c r="A10" s="46" t="s">
+      <c r="A10" s="38" t="s">
         <v>52</v>
       </c>
-      <c r="B10" s="24"/>
-      <c r="C10" s="24"/>
-      <c r="D10" s="24" t="s">
+      <c r="B10" s="39"/>
+      <c r="C10" s="39"/>
+      <c r="D10" s="39" t="s">
         <v>53</v>
       </c>
-      <c r="E10" s="24"/>
-      <c r="F10" s="24"/>
+      <c r="E10" s="39"/>
+      <c r="F10" s="39"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
-      <c r="I10" s="47"/>
-      <c r="J10" s="32"/>
-      <c r="K10" s="32"/>
-      <c r="L10" s="48"/>
+      <c r="I10" s="70"/>
+      <c r="J10" s="71"/>
+      <c r="K10" s="71"/>
+      <c r="L10" s="72"/>
     </row>
     <row r="11" spans="1:23" s="8" customFormat="1" ht="21" customHeight="1">
       <c r="A11" s="12" t="s">
@@ -1552,47 +1538,47 @@
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
-      <c r="D11" s="74" t="s">
+      <c r="D11" s="2" t="s">
         <v>61</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
-      <c r="I11" s="47"/>
-      <c r="J11" s="32"/>
-      <c r="K11" s="32"/>
-      <c r="L11" s="48"/>
+      <c r="I11" s="70"/>
+      <c r="J11" s="71"/>
+      <c r="K11" s="71"/>
+      <c r="L11" s="72"/>
     </row>
     <row r="12" spans="1:23" s="8" customFormat="1" ht="21" customHeight="1">
-      <c r="A12" s="43" t="s">
+      <c r="A12" s="59" t="s">
         <v>54</v>
       </c>
-      <c r="B12" s="31"/>
-      <c r="C12" s="75" t="s">
+      <c r="B12" s="60"/>
+      <c r="C12" s="39" t="s">
         <v>62</v>
       </c>
-      <c r="D12" s="69"/>
-      <c r="E12" s="52" t="s">
+      <c r="D12" s="54"/>
+      <c r="E12" s="34" t="s">
         <v>38</v>
       </c>
-      <c r="F12" s="52"/>
-      <c r="G12" s="52"/>
-      <c r="H12" s="52"/>
-      <c r="I12" s="47"/>
-      <c r="J12" s="32"/>
-      <c r="K12" s="32"/>
-      <c r="L12" s="48"/>
+      <c r="F12" s="34"/>
+      <c r="G12" s="34"/>
+      <c r="H12" s="34"/>
+      <c r="I12" s="70"/>
+      <c r="J12" s="71"/>
+      <c r="K12" s="71"/>
+      <c r="L12" s="72"/>
     </row>
     <row r="13" spans="1:23" s="8" customFormat="1" ht="21" customHeight="1">
-      <c r="A13" s="43" t="s">
+      <c r="A13" s="59" t="s">
         <v>55</v>
       </c>
-      <c r="B13" s="31"/>
-      <c r="C13" s="24" t="s">
+      <c r="B13" s="60"/>
+      <c r="C13" s="39" t="s">
         <v>62</v>
       </c>
-      <c r="D13" s="24"/>
+      <c r="D13" s="39"/>
       <c r="E13" s="18" t="s">
         <v>29</v>
       </c>
@@ -1605,21 +1591,21 @@
       <c r="H13" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="I13" s="47"/>
-      <c r="J13" s="32"/>
-      <c r="K13" s="32"/>
-      <c r="L13" s="48"/>
+      <c r="I13" s="70"/>
+      <c r="J13" s="71"/>
+      <c r="K13" s="71"/>
+      <c r="L13" s="72"/>
     </row>
     <row r="14" spans="1:23" s="8" customFormat="1" ht="21" customHeight="1">
-      <c r="A14" s="43" t="s">
+      <c r="A14" s="59" t="s">
         <v>55</v>
       </c>
-      <c r="B14" s="31"/>
-      <c r="C14" s="24" t="s">
+      <c r="B14" s="60"/>
+      <c r="C14" s="39" t="s">
         <v>62</v>
       </c>
-      <c r="D14" s="24"/>
-      <c r="E14" s="52" t="s">
+      <c r="D14" s="39"/>
+      <c r="E14" s="34" t="s">
         <v>30</v>
       </c>
       <c r="F14" s="18" t="s">
@@ -1627,37 +1613,37 @@
       </c>
       <c r="G14" s="20"/>
       <c r="H14" s="20"/>
-      <c r="I14" s="47"/>
-      <c r="J14" s="32"/>
-      <c r="K14" s="32"/>
-      <c r="L14" s="48"/>
+      <c r="I14" s="70"/>
+      <c r="J14" s="71"/>
+      <c r="K14" s="71"/>
+      <c r="L14" s="72"/>
     </row>
     <row r="15" spans="1:23" s="8" customFormat="1" ht="21" customHeight="1">
-      <c r="A15" s="73" t="s">
+      <c r="A15" s="61" t="s">
         <v>63</v>
       </c>
-      <c r="B15" s="30"/>
-      <c r="C15" s="30"/>
+      <c r="B15" s="62"/>
+      <c r="C15" s="62"/>
       <c r="D15" s="2"/>
-      <c r="E15" s="52"/>
+      <c r="E15" s="34"/>
       <c r="F15" s="18" t="s">
         <v>36</v>
       </c>
       <c r="G15" s="18"/>
       <c r="H15" s="18"/>
-      <c r="I15" s="47"/>
-      <c r="J15" s="32"/>
-      <c r="K15" s="32"/>
-      <c r="L15" s="48"/>
+      <c r="I15" s="70"/>
+      <c r="J15" s="71"/>
+      <c r="K15" s="71"/>
+      <c r="L15" s="72"/>
     </row>
     <row r="16" spans="1:23" s="8" customFormat="1" ht="21" customHeight="1">
-      <c r="A16" s="46" t="s">
+      <c r="A16" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="B16" s="24"/>
-      <c r="C16" s="24"/>
+      <c r="B16" s="39"/>
+      <c r="C16" s="39"/>
       <c r="D16" s="2"/>
-      <c r="E16" s="52" t="s">
+      <c r="E16" s="34" t="s">
         <v>31</v>
       </c>
       <c r="F16" s="18" t="s">
@@ -1665,217 +1651,217 @@
       </c>
       <c r="G16" s="20"/>
       <c r="H16" s="20"/>
-      <c r="I16" s="47"/>
-      <c r="J16" s="32"/>
-      <c r="K16" s="32"/>
-      <c r="L16" s="48"/>
+      <c r="I16" s="70"/>
+      <c r="J16" s="71"/>
+      <c r="K16" s="71"/>
+      <c r="L16" s="72"/>
     </row>
     <row r="17" spans="1:29" s="8" customFormat="1" ht="21" customHeight="1">
-      <c r="A17" s="44" t="s">
+      <c r="A17" s="63" t="s">
         <v>49</v>
       </c>
-      <c r="B17" s="85"/>
-      <c r="C17" s="85"/>
+      <c r="B17" s="41"/>
+      <c r="C17" s="41"/>
       <c r="D17" s="9"/>
-      <c r="E17" s="52"/>
+      <c r="E17" s="34"/>
       <c r="F17" s="18" t="s">
         <v>36</v>
       </c>
       <c r="G17" s="20"/>
       <c r="H17" s="20"/>
-      <c r="I17" s="47"/>
-      <c r="J17" s="32"/>
-      <c r="K17" s="32"/>
-      <c r="L17" s="48"/>
+      <c r="I17" s="70"/>
+      <c r="J17" s="71"/>
+      <c r="K17" s="71"/>
+      <c r="L17" s="72"/>
     </row>
     <row r="18" spans="1:29" s="8" customFormat="1" ht="18.600000000000001" customHeight="1">
-      <c r="A18" s="55"/>
-      <c r="B18" s="56"/>
-      <c r="C18" s="56"/>
-      <c r="D18" s="56"/>
+      <c r="A18" s="50"/>
+      <c r="B18" s="51"/>
+      <c r="C18" s="51"/>
+      <c r="D18" s="51"/>
       <c r="E18" s="13"/>
       <c r="F18" s="14"/>
       <c r="G18" s="13"/>
       <c r="H18" s="13"/>
-      <c r="I18" s="49"/>
-      <c r="J18" s="50"/>
-      <c r="K18" s="50"/>
-      <c r="L18" s="51"/>
+      <c r="I18" s="73"/>
+      <c r="J18" s="74"/>
+      <c r="K18" s="74"/>
+      <c r="L18" s="75"/>
     </row>
     <row r="19" spans="1:29" s="8" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A19" s="38" t="s">
+      <c r="A19" s="64" t="s">
         <v>4</v>
       </c>
-      <c r="B19" s="39"/>
-      <c r="C19" s="39"/>
-      <c r="D19" s="39"/>
-      <c r="E19" s="39"/>
-      <c r="F19" s="39"/>
-      <c r="G19" s="39"/>
-      <c r="H19" s="39"/>
-      <c r="I19" s="57" t="s">
+      <c r="B19" s="65"/>
+      <c r="C19" s="65"/>
+      <c r="D19" s="65"/>
+      <c r="E19" s="65"/>
+      <c r="F19" s="65"/>
+      <c r="G19" s="65"/>
+      <c r="H19" s="65"/>
+      <c r="I19" s="66" t="s">
         <v>2</v>
       </c>
-      <c r="J19" s="58"/>
-      <c r="K19" s="58"/>
-      <c r="L19" s="59"/>
+      <c r="J19" s="67"/>
+      <c r="K19" s="67"/>
+      <c r="L19" s="68"/>
     </row>
     <row r="20" spans="1:29" s="8" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A20" s="53" t="s">
+      <c r="A20" s="43" t="s">
         <v>37</v>
       </c>
-      <c r="B20" s="28"/>
-      <c r="C20" s="28"/>
-      <c r="D20" s="28"/>
-      <c r="E20" s="28"/>
-      <c r="F20" s="28"/>
-      <c r="G20" s="28"/>
-      <c r="H20" s="29"/>
-      <c r="I20" s="53"/>
-      <c r="J20" s="28"/>
-      <c r="K20" s="28"/>
-      <c r="L20" s="54"/>
-      <c r="S20" s="37"/>
-      <c r="T20" s="37"/>
-      <c r="U20" s="37"/>
-      <c r="V20" s="37"/>
-      <c r="W20" s="37"/>
-      <c r="X20" s="37"/>
+      <c r="B20" s="27"/>
+      <c r="C20" s="27"/>
+      <c r="D20" s="27"/>
+      <c r="E20" s="27"/>
+      <c r="F20" s="27"/>
+      <c r="G20" s="27"/>
+      <c r="H20" s="69"/>
+      <c r="I20" s="43"/>
+      <c r="J20" s="27"/>
+      <c r="K20" s="27"/>
+      <c r="L20" s="44"/>
+      <c r="S20" s="58"/>
+      <c r="T20" s="58"/>
+      <c r="U20" s="58"/>
+      <c r="V20" s="58"/>
+      <c r="W20" s="58"/>
+      <c r="X20" s="58"/>
     </row>
     <row r="21" spans="1:29" s="8" customFormat="1" ht="21" customHeight="1">
-      <c r="A21" s="46" t="s">
+      <c r="A21" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="B21" s="24"/>
-      <c r="C21" s="24"/>
-      <c r="D21" s="24"/>
-      <c r="E21" s="24"/>
-      <c r="F21" s="24"/>
-      <c r="G21" s="24"/>
-      <c r="H21" s="24"/>
-      <c r="I21" s="53"/>
-      <c r="J21" s="28"/>
-      <c r="K21" s="28"/>
-      <c r="L21" s="54"/>
-      <c r="S21" s="37"/>
-      <c r="T21" s="37"/>
-      <c r="U21" s="37"/>
-      <c r="V21" s="37"/>
-      <c r="W21" s="37"/>
-      <c r="X21" s="37"/>
+      <c r="B21" s="39"/>
+      <c r="C21" s="39"/>
+      <c r="D21" s="39"/>
+      <c r="E21" s="39"/>
+      <c r="F21" s="39"/>
+      <c r="G21" s="39"/>
+      <c r="H21" s="39"/>
+      <c r="I21" s="43"/>
+      <c r="J21" s="27"/>
+      <c r="K21" s="27"/>
+      <c r="L21" s="44"/>
+      <c r="S21" s="58"/>
+      <c r="T21" s="58"/>
+      <c r="U21" s="58"/>
+      <c r="V21" s="58"/>
+      <c r="W21" s="58"/>
+      <c r="X21" s="58"/>
     </row>
     <row r="22" spans="1:29" s="8" customFormat="1" ht="21.75" customHeight="1">
-      <c r="A22" s="46" t="s">
+      <c r="A22" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="B22" s="24"/>
-      <c r="C22" s="24"/>
-      <c r="D22" s="24"/>
-      <c r="E22" s="24"/>
-      <c r="F22" s="24"/>
-      <c r="G22" s="24"/>
-      <c r="H22" s="24"/>
-      <c r="I22" s="53"/>
-      <c r="J22" s="28"/>
-      <c r="K22" s="28"/>
-      <c r="L22" s="54"/>
+      <c r="B22" s="39"/>
+      <c r="C22" s="39"/>
+      <c r="D22" s="39"/>
+      <c r="E22" s="39"/>
+      <c r="F22" s="39"/>
+      <c r="G22" s="39"/>
+      <c r="H22" s="39"/>
+      <c r="I22" s="43"/>
+      <c r="J22" s="27"/>
+      <c r="K22" s="27"/>
+      <c r="L22" s="44"/>
     </row>
     <row r="23" spans="1:29" s="8" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A23" s="46" t="s">
+      <c r="A23" s="38" t="s">
         <v>40</v>
       </c>
-      <c r="B23" s="24"/>
-      <c r="C23" s="24"/>
-      <c r="D23" s="24"/>
-      <c r="E23" s="24"/>
-      <c r="F23" s="24"/>
-      <c r="G23" s="24"/>
-      <c r="H23" s="24"/>
-      <c r="I23" s="77" t="s">
+      <c r="B23" s="39"/>
+      <c r="C23" s="39"/>
+      <c r="D23" s="39"/>
+      <c r="E23" s="39"/>
+      <c r="F23" s="39"/>
+      <c r="G23" s="39"/>
+      <c r="H23" s="39"/>
+      <c r="I23" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="J23" s="26"/>
-      <c r="K23" s="26"/>
-      <c r="L23" s="45"/>
+      <c r="J23" s="41"/>
+      <c r="K23" s="41"/>
+      <c r="L23" s="42"/>
     </row>
     <row r="24" spans="1:29" s="8" customFormat="1" ht="21" customHeight="1">
-      <c r="A24" s="46" t="s">
+      <c r="A24" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="B24" s="24"/>
-      <c r="C24" s="24"/>
-      <c r="D24" s="24"/>
-      <c r="E24" s="24"/>
-      <c r="F24" s="24"/>
-      <c r="G24" s="24"/>
-      <c r="H24" s="24"/>
-      <c r="I24" s="53"/>
-      <c r="J24" s="28"/>
-      <c r="K24" s="28"/>
-      <c r="L24" s="54"/>
+      <c r="B24" s="39"/>
+      <c r="C24" s="39"/>
+      <c r="D24" s="39"/>
+      <c r="E24" s="39"/>
+      <c r="F24" s="39"/>
+      <c r="G24" s="39"/>
+      <c r="H24" s="39"/>
+      <c r="I24" s="43"/>
+      <c r="J24" s="27"/>
+      <c r="K24" s="27"/>
+      <c r="L24" s="44"/>
     </row>
     <row r="25" spans="1:29" s="8" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A25" s="46" t="s">
+      <c r="A25" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="B25" s="24"/>
-      <c r="C25" s="24"/>
-      <c r="D25" s="24"/>
-      <c r="E25" s="24"/>
-      <c r="F25" s="24"/>
-      <c r="G25" s="24"/>
-      <c r="H25" s="24"/>
-      <c r="I25" s="53"/>
-      <c r="J25" s="28"/>
-      <c r="K25" s="28"/>
-      <c r="L25" s="54"/>
+      <c r="B25" s="39"/>
+      <c r="C25" s="39"/>
+      <c r="D25" s="39"/>
+      <c r="E25" s="39"/>
+      <c r="F25" s="39"/>
+      <c r="G25" s="39"/>
+      <c r="H25" s="39"/>
+      <c r="I25" s="43"/>
+      <c r="J25" s="27"/>
+      <c r="K25" s="27"/>
+      <c r="L25" s="44"/>
       <c r="AC25" s="10"/>
     </row>
     <row r="26" spans="1:29" s="8" customFormat="1" ht="21" customHeight="1">
-      <c r="A26" s="46" t="s">
+      <c r="A26" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="B26" s="24"/>
-      <c r="C26" s="24"/>
-      <c r="D26" s="24"/>
-      <c r="E26" s="24"/>
-      <c r="F26" s="24"/>
-      <c r="G26" s="24"/>
-      <c r="H26" s="24"/>
-      <c r="I26" s="53"/>
-      <c r="J26" s="28"/>
-      <c r="K26" s="28"/>
-      <c r="L26" s="54"/>
+      <c r="B26" s="39"/>
+      <c r="C26" s="39"/>
+      <c r="D26" s="39"/>
+      <c r="E26" s="39"/>
+      <c r="F26" s="39"/>
+      <c r="G26" s="39"/>
+      <c r="H26" s="39"/>
+      <c r="I26" s="43"/>
+      <c r="J26" s="27"/>
+      <c r="K26" s="27"/>
+      <c r="L26" s="44"/>
     </row>
     <row r="27" spans="1:29" s="8" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A27" s="66" t="s">
+      <c r="A27" s="48" t="s">
         <v>45</v>
       </c>
-      <c r="B27" s="35"/>
-      <c r="C27" s="35"/>
-      <c r="D27" s="35"/>
-      <c r="E27" s="35"/>
-      <c r="F27" s="35"/>
-      <c r="G27" s="35"/>
-      <c r="H27" s="35"/>
-      <c r="I27" s="53"/>
-      <c r="J27" s="28"/>
-      <c r="K27" s="28"/>
-      <c r="L27" s="54"/>
+      <c r="B27" s="49"/>
+      <c r="C27" s="49"/>
+      <c r="D27" s="49"/>
+      <c r="E27" s="49"/>
+      <c r="F27" s="49"/>
+      <c r="G27" s="49"/>
+      <c r="H27" s="49"/>
+      <c r="I27" s="43"/>
+      <c r="J27" s="27"/>
+      <c r="K27" s="27"/>
+      <c r="L27" s="44"/>
     </row>
     <row r="28" spans="1:29" s="8" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A28" s="55"/>
-      <c r="B28" s="56"/>
-      <c r="C28" s="56"/>
-      <c r="D28" s="56"/>
-      <c r="E28" s="56"/>
-      <c r="F28" s="56"/>
-      <c r="G28" s="56"/>
-      <c r="H28" s="56"/>
-      <c r="I28" s="63"/>
-      <c r="J28" s="64"/>
-      <c r="K28" s="64"/>
-      <c r="L28" s="65"/>
+      <c r="A28" s="50"/>
+      <c r="B28" s="51"/>
+      <c r="C28" s="51"/>
+      <c r="D28" s="51"/>
+      <c r="E28" s="51"/>
+      <c r="F28" s="51"/>
+      <c r="G28" s="51"/>
+      <c r="H28" s="51"/>
+      <c r="I28" s="45"/>
+      <c r="J28" s="46"/>
+      <c r="K28" s="46"/>
+      <c r="L28" s="47"/>
     </row>
     <row r="29" spans="1:29" s="8" customFormat="1" ht="27.75" customHeight="1">
       <c r="A29" s="15"/>
@@ -1888,77 +1874,77 @@
       <c r="F29" s="16"/>
       <c r="G29" s="16"/>
       <c r="H29" s="16"/>
-      <c r="I29" s="67" t="s">
+      <c r="I29" s="52" t="s">
         <v>9</v>
       </c>
-      <c r="J29" s="67"/>
-      <c r="K29" s="67"/>
-      <c r="L29" s="68"/>
+      <c r="J29" s="52"/>
+      <c r="K29" s="52"/>
+      <c r="L29" s="53"/>
     </row>
     <row r="30" spans="1:29" s="8" customFormat="1" ht="21.75" customHeight="1">
-      <c r="A30" s="46" t="s">
+      <c r="A30" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="B30" s="24"/>
-      <c r="C30" s="24"/>
-      <c r="D30" s="24"/>
-      <c r="E30" s="24"/>
-      <c r="F30" s="24"/>
-      <c r="G30" s="24"/>
-      <c r="H30" s="24"/>
-      <c r="I30" s="24"/>
-      <c r="J30" s="24"/>
-      <c r="K30" s="24"/>
-      <c r="L30" s="69"/>
+      <c r="B30" s="39"/>
+      <c r="C30" s="39"/>
+      <c r="D30" s="39"/>
+      <c r="E30" s="39"/>
+      <c r="F30" s="39"/>
+      <c r="G30" s="39"/>
+      <c r="H30" s="39"/>
+      <c r="I30" s="39"/>
+      <c r="J30" s="39"/>
+      <c r="K30" s="39"/>
+      <c r="L30" s="54"/>
     </row>
     <row r="31" spans="1:29" s="8" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A31" s="25" t="s">
+      <c r="A31" s="55" t="s">
         <v>46</v>
       </c>
-      <c r="B31" s="26"/>
-      <c r="C31" s="26"/>
-      <c r="D31" s="26"/>
-      <c r="E31" s="26"/>
-      <c r="F31" s="26"/>
-      <c r="G31" s="26"/>
-      <c r="H31" s="26"/>
-      <c r="I31" s="36" t="s">
+      <c r="B31" s="41"/>
+      <c r="C31" s="41"/>
+      <c r="D31" s="41"/>
+      <c r="E31" s="41"/>
+      <c r="F31" s="41"/>
+      <c r="G31" s="41"/>
+      <c r="H31" s="41"/>
+      <c r="I31" s="56" t="s">
         <v>11</v>
       </c>
-      <c r="J31" s="26"/>
-      <c r="K31" s="26" t="s">
+      <c r="J31" s="41"/>
+      <c r="K31" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="L31" s="27"/>
+      <c r="L31" s="57"/>
     </row>
     <row r="32" spans="1:29" s="8" customFormat="1" ht="18.600000000000001" customHeight="1">
-      <c r="A32" s="60" t="s">
+      <c r="A32" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="B32" s="61"/>
-      <c r="C32" s="61"/>
-      <c r="D32" s="61"/>
-      <c r="E32" s="61"/>
-      <c r="F32" s="61"/>
-      <c r="G32" s="61"/>
-      <c r="H32" s="61"/>
-      <c r="I32" s="61"/>
-      <c r="J32" s="61"/>
-      <c r="K32" s="61"/>
-      <c r="L32" s="62"/>
-    </row>
-    <row r="33" spans="1:14" s="8" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A33" s="70" t="s">
+      <c r="B32" s="36"/>
+      <c r="C32" s="36"/>
+      <c r="D32" s="36"/>
+      <c r="E32" s="36"/>
+      <c r="F32" s="36"/>
+      <c r="G32" s="36"/>
+      <c r="H32" s="36"/>
+      <c r="I32" s="36"/>
+      <c r="J32" s="36"/>
+      <c r="K32" s="36"/>
+      <c r="L32" s="37"/>
+    </row>
+    <row r="33" spans="1:13" s="8" customFormat="1" ht="18.75" customHeight="1">
+      <c r="A33" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="B33" s="70"/>
+      <c r="B33" s="33"/>
       <c r="C33" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="D33" s="52" t="s">
+      <c r="D33" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="E33" s="52"/>
+      <c r="E33" s="34"/>
       <c r="F33" s="18" t="s">
         <v>17</v>
       </c>
@@ -1971,22 +1957,22 @@
       <c r="I33" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="J33" s="52" t="s">
+      <c r="J33" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="K33" s="52"/>
-      <c r="L33" s="52"/>
-    </row>
-    <row r="34" spans="1:14" s="8" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A34" s="70"/>
-      <c r="B34" s="70"/>
+      <c r="K33" s="34"/>
+      <c r="L33" s="34"/>
+    </row>
+    <row r="34" spans="1:13" s="8" customFormat="1" ht="18.75" customHeight="1">
+      <c r="A34" s="33"/>
+      <c r="B34" s="33"/>
       <c r="C34" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="D34" s="52" t="s">
+      <c r="D34" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="E34" s="52"/>
+      <c r="E34" s="34"/>
       <c r="F34" s="18" t="s">
         <v>19</v>
       </c>
@@ -1999,20 +1985,20 @@
       <c r="I34" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="J34" s="52"/>
-      <c r="K34" s="52"/>
-      <c r="L34" s="52"/>
-    </row>
-    <row r="35" spans="1:14" s="10" customFormat="1" ht="24.75" customHeight="1">
-      <c r="A35" s="71" t="s">
+      <c r="J34" s="34"/>
+      <c r="K34" s="34"/>
+      <c r="L34" s="34"/>
+    </row>
+    <row r="35" spans="1:13" s="10" customFormat="1" ht="24.75" customHeight="1">
+      <c r="A35" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="B35" s="71"/>
+      <c r="B35" s="30"/>
       <c r="C35" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="D35" s="71"/>
-      <c r="E35" s="71"/>
+      <c r="D35" s="30"/>
+      <c r="E35" s="30"/>
       <c r="F35" s="19" t="s">
         <v>22</v>
       </c>
@@ -2021,24 +2007,23 @@
         <v>23</v>
       </c>
       <c r="I35" s="20"/>
-      <c r="J35" s="80" t="s">
+      <c r="J35" s="23" t="s">
         <v>69</v>
       </c>
       <c r="K35" s="1"/>
-      <c r="L35" s="83"/>
-      <c r="M35" s="81"/>
-      <c r="N35" s="82"/>
-    </row>
-    <row r="36" spans="1:14" s="10" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A36" s="71" t="s">
+      <c r="L35" s="24"/>
+      <c r="M35" s="1"/>
+    </row>
+    <row r="36" spans="1:13" s="10" customFormat="1" ht="20.25" customHeight="1">
+      <c r="A36" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="B36" s="71"/>
+      <c r="B36" s="30"/>
       <c r="C36" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="D36" s="71"/>
-      <c r="E36" s="71"/>
+      <c r="D36" s="30"/>
+      <c r="E36" s="30"/>
       <c r="F36" s="19" t="s">
         <v>25</v>
       </c>
@@ -2047,20 +2032,20 @@
         <v>26</v>
       </c>
       <c r="I36" s="20"/>
-      <c r="J36" s="72"/>
-      <c r="K36" s="72"/>
-      <c r="L36" s="72"/>
-    </row>
-    <row r="37" spans="1:14" s="10" customFormat="1" ht="21" customHeight="1">
-      <c r="A37" s="71" t="s">
+      <c r="J36" s="31"/>
+      <c r="K36" s="31"/>
+      <c r="L36" s="31"/>
+    </row>
+    <row r="37" spans="1:13" s="10" customFormat="1" ht="21" customHeight="1">
+      <c r="A37" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="B37" s="71"/>
+      <c r="B37" s="30"/>
       <c r="C37" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="D37" s="71"/>
-      <c r="E37" s="71"/>
+      <c r="D37" s="30"/>
+      <c r="E37" s="30"/>
       <c r="F37" s="19" t="s">
         <v>27</v>
       </c>
@@ -2069,27 +2054,27 @@
         <v>27</v>
       </c>
       <c r="I37" s="20"/>
-      <c r="J37" s="72"/>
-      <c r="K37" s="72"/>
-      <c r="L37" s="72"/>
-    </row>
-    <row r="38" spans="1:14" s="8" customFormat="1" ht="28.5" customHeight="1">
-      <c r="A38" s="23" t="s">
+      <c r="J37" s="31"/>
+      <c r="K37" s="31"/>
+      <c r="L37" s="31"/>
+    </row>
+    <row r="38" spans="1:13" s="8" customFormat="1" ht="28.5" customHeight="1">
+      <c r="A38" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="B38" s="23"/>
-      <c r="C38" s="23"/>
-      <c r="D38" s="23"/>
-      <c r="E38" s="23"/>
-      <c r="F38" s="23"/>
-      <c r="G38" s="23"/>
-      <c r="H38" s="23"/>
-      <c r="I38" s="23"/>
-      <c r="J38" s="23"/>
-      <c r="K38" s="23"/>
-      <c r="L38" s="23"/>
-    </row>
-    <row r="39" spans="1:14" s="8" customFormat="1" ht="23.25" customHeight="1">
+      <c r="B38" s="32"/>
+      <c r="C38" s="32"/>
+      <c r="D38" s="32"/>
+      <c r="E38" s="32"/>
+      <c r="F38" s="32"/>
+      <c r="G38" s="32"/>
+      <c r="H38" s="32"/>
+      <c r="I38" s="32"/>
+      <c r="J38" s="32"/>
+      <c r="K38" s="32"/>
+      <c r="L38" s="32"/>
+    </row>
+    <row r="39" spans="1:13" s="8" customFormat="1" ht="23.25" customHeight="1">
       <c r="A39" s="2" t="s">
         <v>67</v>
       </c>
@@ -2101,11 +2086,11 @@
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
       <c r="I39" s="2"/>
-      <c r="J39" s="28"/>
-      <c r="K39" s="28"/>
-      <c r="L39" s="28"/>
-    </row>
-    <row r="40" spans="1:14" s="8" customFormat="1" ht="23.25" customHeight="1">
+      <c r="J39" s="27"/>
+      <c r="K39" s="27"/>
+      <c r="L39" s="27"/>
+    </row>
+    <row r="40" spans="1:13" s="8" customFormat="1" ht="23.25" customHeight="1">
       <c r="A40" s="2" t="s">
         <v>66</v>
       </c>
@@ -2117,11 +2102,11 @@
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
       <c r="I40" s="2"/>
-      <c r="J40" s="28"/>
-      <c r="K40" s="28"/>
-      <c r="L40" s="28"/>
-    </row>
-    <row r="41" spans="1:14" s="8" customFormat="1" ht="23.4">
+      <c r="J40" s="27"/>
+      <c r="K40" s="27"/>
+      <c r="L40" s="27"/>
+    </row>
+    <row r="41" spans="1:13" s="8" customFormat="1" ht="23.4">
       <c r="A41" s="2" t="s">
         <v>68</v>
       </c>
@@ -2133,11 +2118,11 @@
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
       <c r="I41" s="2"/>
-      <c r="J41" s="28"/>
-      <c r="K41" s="28"/>
-      <c r="L41" s="28"/>
-    </row>
-    <row r="42" spans="1:14" s="8" customFormat="1" ht="21.75" customHeight="1">
+      <c r="J41" s="27"/>
+      <c r="K41" s="27"/>
+      <c r="L41" s="27"/>
+    </row>
+    <row r="42" spans="1:13" s="8" customFormat="1" ht="21.75" customHeight="1">
       <c r="A42" s="3"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
@@ -2147,13 +2132,13 @@
       <c r="G42" s="3"/>
       <c r="H42" s="4"/>
       <c r="I42" s="11"/>
-      <c r="J42" s="86" t="s">
+      <c r="J42" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="K42" s="86"/>
-      <c r="L42" s="86"/>
-    </row>
-    <row r="43" spans="1:14" s="8" customFormat="1" ht="16.95" customHeight="1">
+      <c r="K42" s="28"/>
+      <c r="L42" s="28"/>
+    </row>
+    <row r="43" spans="1:13" s="8" customFormat="1" ht="16.95" customHeight="1">
       <c r="A43" s="4"/>
       <c r="B43" s="4"/>
       <c r="C43" s="4"/>
@@ -2162,20 +2147,20 @@
       <c r="F43" s="4"/>
       <c r="G43" s="4"/>
       <c r="H43" s="4"/>
-      <c r="I43" s="22"/>
-      <c r="J43" s="22"/>
-      <c r="K43" s="22"/>
+      <c r="I43" s="29"/>
+      <c r="J43" s="29"/>
+      <c r="K43" s="29"/>
       <c r="L43" s="4"/>
     </row>
-    <row r="44" spans="1:14" ht="16.95" customHeight="1">
-      <c r="I44" s="22"/>
-      <c r="J44" s="22"/>
-      <c r="K44" s="22"/>
-    </row>
-    <row r="46" spans="1:14" ht="16.95" customHeight="1">
-      <c r="I46" s="22"/>
-      <c r="J46" s="22"/>
-      <c r="K46" s="22"/>
+    <row r="44" spans="1:13" ht="16.95" customHeight="1">
+      <c r="I44" s="29"/>
+      <c r="J44" s="29"/>
+      <c r="K44" s="29"/>
+    </row>
+    <row r="46" spans="1:13" ht="16.95" customHeight="1">
+      <c r="I46" s="29"/>
+      <c r="J46" s="29"/>
+      <c r="K46" s="29"/>
     </row>
     <row r="67" spans="1:12" s="3" customFormat="1" ht="16.95" customHeight="1">
       <c r="A67" s="4"/>
@@ -2193,56 +2178,12 @@
     </row>
   </sheetData>
   <mergeCells count="68">
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="J42:L42"/>
-    <mergeCell ref="I43:K43"/>
-    <mergeCell ref="I44:K44"/>
-    <mergeCell ref="I46:K46"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="J36:L37"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="A38:L38"/>
-    <mergeCell ref="J39:L41"/>
-    <mergeCell ref="A33:B34"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="J33:L34"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="A32:L32"/>
-    <mergeCell ref="A23:H23"/>
-    <mergeCell ref="I23:L23"/>
-    <mergeCell ref="A24:H24"/>
-    <mergeCell ref="I24:L28"/>
-    <mergeCell ref="A25:H25"/>
-    <mergeCell ref="A26:H26"/>
-    <mergeCell ref="A27:H27"/>
-    <mergeCell ref="A28:H28"/>
-    <mergeCell ref="I29:L29"/>
-    <mergeCell ref="A30:L30"/>
-    <mergeCell ref="A31:H31"/>
-    <mergeCell ref="I31:J31"/>
-    <mergeCell ref="K31:L31"/>
-    <mergeCell ref="S20:X21"/>
-    <mergeCell ref="A21:H21"/>
-    <mergeCell ref="I21:L22"/>
-    <mergeCell ref="A22:H22"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="A17:C17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="A19:H19"/>
-    <mergeCell ref="I19:L20"/>
-    <mergeCell ref="A20:H20"/>
+    <mergeCell ref="J1:L2"/>
+    <mergeCell ref="J3:L3"/>
+    <mergeCell ref="A4:L4"/>
+    <mergeCell ref="A6:H6"/>
+    <mergeCell ref="I6:L6"/>
+    <mergeCell ref="D1:G2"/>
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="C13:D13"/>
     <mergeCell ref="R6:W7"/>
@@ -2255,12 +2196,56 @@
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="C12:D12"/>
     <mergeCell ref="E12:H12"/>
-    <mergeCell ref="J1:L2"/>
-    <mergeCell ref="J3:L3"/>
-    <mergeCell ref="A4:L4"/>
-    <mergeCell ref="A6:H6"/>
-    <mergeCell ref="I6:L6"/>
-    <mergeCell ref="D1:G2"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="A19:H19"/>
+    <mergeCell ref="I19:L20"/>
+    <mergeCell ref="A20:H20"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="A30:L30"/>
+    <mergeCell ref="A31:H31"/>
+    <mergeCell ref="I31:J31"/>
+    <mergeCell ref="K31:L31"/>
+    <mergeCell ref="S20:X21"/>
+    <mergeCell ref="A21:H21"/>
+    <mergeCell ref="I21:L22"/>
+    <mergeCell ref="A22:H22"/>
+    <mergeCell ref="A25:H25"/>
+    <mergeCell ref="A26:H26"/>
+    <mergeCell ref="A27:H27"/>
+    <mergeCell ref="A28:H28"/>
+    <mergeCell ref="I29:L29"/>
+    <mergeCell ref="I44:K44"/>
+    <mergeCell ref="I46:K46"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="J36:L37"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="A38:L38"/>
+    <mergeCell ref="J39:L41"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="J42:L42"/>
+    <mergeCell ref="I43:K43"/>
+    <mergeCell ref="A33:B34"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="J33:L34"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="A32:L32"/>
+    <mergeCell ref="A23:H23"/>
+    <mergeCell ref="I23:L23"/>
+    <mergeCell ref="A24:H24"/>
+    <mergeCell ref="I24:L28"/>
   </mergeCells>
   <pageMargins left="0.55118110236220474" right="0.23622047244094491" top="0.35433070866141736" bottom="0.35433070866141736" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="88" orientation="portrait" horizontalDpi="4294967293" verticalDpi="300" r:id="rId1"/>

</xml_diff>